<commit_message>
change subject to subject_topic
</commit_message>
<xml_diff>
--- a/metadata_templates/HP_image_metadata_template.xlsx
+++ b/metadata_templates/HP_image_metadata_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelbolam/Documents/GitHub/MAD_Islandora_Metadata/islandora_metadata/metadata_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788C734A-CCD4-AC48-BB25-55CD040EA340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6BC1B0-5153-CB47-BD8F-54F0544FA504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1100" windowWidth="22580" windowHeight="14900" xr2:uid="{E3B8F13D-DE85-3546-8BD7-9AF08846EFCA}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>creator</t>
   </si>
   <si>
-    <t>subject</t>
-  </si>
-  <si>
     <t>type_of_resource</t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>source_collection_id</t>
+  </si>
+  <si>
+    <t>subject_topic</t>
   </si>
 </sst>
 </file>
@@ -502,37 +502,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF09D21-D64E-6B44-B18F-A136418E42A3}">
   <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="80.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="80.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="54.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="10.5" style="1" customWidth="1"/>
-    <col min="20" max="21" width="16.33203125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="80.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="80.6640625" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="20" width="17.33203125" style="1"/>
+    <col min="21" max="21" width="20.33203125" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="17.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -540,70 +521,70 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="W1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>